<commit_message>
fixed bug caused by mutable default parameters and rest sector calculation works
</commit_message>
<xml_diff>
--- a/output/endemo2_specific_consumption_projections.xlsx
+++ b/output/endemo2_specific_consumption_projections.xlsx
@@ -4633,10 +4633,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1.39</v>
+        <v>1.58</v>
       </c>
       <c r="C2" t="n">
-        <v>6.13</v>
+        <v>7.48</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -4652,10 +4652,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1.39</v>
+        <v>1.38</v>
       </c>
       <c r="C3" t="n">
-        <v>6.13</v>
+        <v>8.34</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
@@ -4690,10 +4690,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1.39</v>
+        <v>2.45</v>
       </c>
       <c r="C5" t="n">
-        <v>6.13</v>
+        <v>4.62</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
@@ -4728,10 +4728,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1.39</v>
+        <v>2.97</v>
       </c>
       <c r="C7" t="n">
-        <v>6.13</v>
+        <v>8.94</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
@@ -4747,10 +4747,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1.39</v>
+        <v>1.34</v>
       </c>
       <c r="C8" t="n">
-        <v>6.13</v>
+        <v>5.71</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
@@ -4766,10 +4766,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1.39</v>
+        <v>1.29</v>
       </c>
       <c r="C9" t="n">
-        <v>6.13</v>
+        <v>6.28</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
@@ -4785,10 +4785,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1.39</v>
+        <v>1.44</v>
       </c>
       <c r="C10" t="n">
-        <v>6.13</v>
+        <v>6.75</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
@@ -4804,10 +4804,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1.39</v>
+        <v>2.15</v>
       </c>
       <c r="C11" t="n">
-        <v>6.13</v>
+        <v>7.83</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
@@ -4823,10 +4823,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1.39</v>
+        <v>1.13</v>
       </c>
       <c r="C12" t="n">
-        <v>6.13</v>
+        <v>5.99</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
@@ -4842,10 +4842,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1.39</v>
+        <v>3.38</v>
       </c>
       <c r="C13" t="n">
-        <v>6.13</v>
+        <v>10.32</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
@@ -4880,10 +4880,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1.39</v>
+        <v>1.9</v>
       </c>
       <c r="C15" t="n">
-        <v>6.13</v>
+        <v>7.02</v>
       </c>
       <c r="D15" t="n">
         <v>0</v>
@@ -4937,10 +4937,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1.39</v>
+        <v>1.69</v>
       </c>
       <c r="C18" t="n">
-        <v>6.13</v>
+        <v>6.22</v>
       </c>
       <c r="D18" t="n">
         <v>0</v>
@@ -4956,10 +4956,10 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>1.39</v>
+        <v>1.1</v>
       </c>
       <c r="C19" t="n">
-        <v>6.13</v>
+        <v>5.74</v>
       </c>
       <c r="D19" t="n">
         <v>0</v>
@@ -4975,10 +4975,10 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1.39</v>
+        <v>1.18</v>
       </c>
       <c r="C20" t="n">
-        <v>6.13</v>
+        <v>7.16</v>
       </c>
       <c r="D20" t="n">
         <v>0</v>
@@ -4994,10 +4994,10 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1.39</v>
+        <v>3.36</v>
       </c>
       <c r="C21" t="n">
-        <v>6.13</v>
+        <v>4.31</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
@@ -5013,10 +5013,10 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>1.39</v>
+        <v>2.36</v>
       </c>
       <c r="C22" t="n">
-        <v>6.13</v>
+        <v>7.02</v>
       </c>
       <c r="D22" t="n">
         <v>0</v>
@@ -5032,10 +5032,10 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>1.39</v>
+        <v>2.25</v>
       </c>
       <c r="C23" t="n">
-        <v>6.13</v>
+        <v>6.4</v>
       </c>
       <c r="D23" t="n">
         <v>0</v>
@@ -5051,10 +5051,10 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>1.39</v>
+        <v>1.91</v>
       </c>
       <c r="C24" t="n">
-        <v>6.13</v>
+        <v>5.94</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>
@@ -5070,10 +5070,10 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>1.39</v>
+        <v>1.28</v>
       </c>
       <c r="C25" t="n">
-        <v>6.13</v>
+        <v>6.01</v>
       </c>
       <c r="D25" t="n">
         <v>0</v>
@@ -5184,10 +5184,10 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>1.39</v>
+        <v>0.99</v>
       </c>
       <c r="C31" t="n">
-        <v>6.13</v>
+        <v>5.41</v>
       </c>
       <c r="D31" t="n">
         <v>0</v>
@@ -5241,10 +5241,10 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>1.39</v>
+        <v>3.38</v>
       </c>
       <c r="C34" t="n">
-        <v>6.13</v>
+        <v>4.12</v>
       </c>
       <c r="D34" t="n">
         <v>0</v>
@@ -5260,10 +5260,10 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>1.39</v>
+        <v>0.99</v>
       </c>
       <c r="C35" t="n">
-        <v>6.13</v>
+        <v>5.41</v>
       </c>
       <c r="D35" t="n">
         <v>0</v>

</xml_diff>